<commit_message>
add res boundary attack for SEED 123
</commit_message>
<xml_diff>
--- a/results/SEED_123/result.xlsx
+++ b/results/SEED_123/result.xlsx
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR12"/>
+  <dimension ref="A1:AZ12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -558,6 +558,18 @@
       <c r="AP1" s="1" t="n"/>
       <c r="AQ1" s="1" t="n"/>
       <c r="AR1" s="1" t="n"/>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>BOUNDARY</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="n"/>
+      <c r="AU1" s="1" t="n"/>
+      <c r="AV1" s="1" t="n"/>
+      <c r="AW1" s="1" t="n"/>
+      <c r="AX1" s="1" t="n"/>
+      <c r="AY1" s="1" t="n"/>
+      <c r="AZ1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="B2" s="1" t="inlineStr">
@@ -775,6 +787,46 @@
           <t>0.20</t>
         </is>
       </c>
+      <c r="AS2" s="1" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="AT2" s="1" t="inlineStr">
+        <is>
+          <t>0.02</t>
+        </is>
+      </c>
+      <c r="AU2" s="1" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="AV2" s="1" t="inlineStr">
+        <is>
+          <t>0.04</t>
+        </is>
+      </c>
+      <c r="AW2" s="1" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="AX2" s="1" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="AY2" s="1" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="AZ2" s="1" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -924,6 +976,30 @@
       </c>
       <c r="AR4" t="n">
         <v>30.89287757873535</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>4.272983551025391</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>4.301231384277344</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>4.329296588897705</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>4.438754081726074</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>4.507856845855713</v>
+      </c>
+      <c r="AX4" t="n">
+        <v>4.69865608215332</v>
+      </c>
+      <c r="AY4" t="n">
+        <v>5.214001655578613</v>
+      </c>
+      <c r="AZ4" t="n">
+        <v>7.47571849822998</v>
       </c>
     </row>
     <row r="5">
@@ -1059,6 +1135,30 @@
       <c r="AR5" t="n">
         <v>31.13849148329875</v>
       </c>
+      <c r="AS5" t="n">
+        <v>5.394301424095979</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>5.420806163785238</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>5.424090106091888</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>5.583747317021231</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>5.663730122252037</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>5.884951340726178</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>6.496286945601298</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>9.275691464706957</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
@@ -1193,6 +1293,30 @@
       <c r="AR6" t="n">
         <v>0.9856417179107666</v>
       </c>
+      <c r="AS6" t="n">
+        <v>0.9996333122253418</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>0.9996324777603149</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>0.9996344447135925</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>0.9996020197868347</v>
+      </c>
+      <c r="AW6" t="n">
+        <v>0.9995958805084229</v>
+      </c>
+      <c r="AX6" t="n">
+        <v>0.9995558261871338</v>
+      </c>
+      <c r="AY6" t="n">
+        <v>0.9994837641716003</v>
+      </c>
+      <c r="AZ6" t="n">
+        <v>0.9988046884536743</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1330,6 +1454,30 @@
       </c>
       <c r="AR7" t="n">
         <v>37.93888092041016</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>4.53721284866333</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>4.605648994445801</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>4.710145950317383</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>4.765591144561768</v>
+      </c>
+      <c r="AW7" t="n">
+        <v>4.971255779266357</v>
+      </c>
+      <c r="AX7" t="n">
+        <v>5.517040729522705</v>
+      </c>
+      <c r="AY7" t="n">
+        <v>6.681266784667969</v>
+      </c>
+      <c r="AZ7" t="n">
+        <v>10.27185726165771</v>
       </c>
     </row>
     <row r="8">
@@ -1465,6 +1613,30 @@
       <c r="AR8" t="n">
         <v>38.09623498611362</v>
       </c>
+      <c r="AS8" t="n">
+        <v>5.610819935981184</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>5.684818180501583</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>5.798989951219583</v>
+      </c>
+      <c r="AV8" t="n">
+        <v>5.841578442192578</v>
+      </c>
+      <c r="AW8" t="n">
+        <v>6.096368002329274</v>
+      </c>
+      <c r="AX8" t="n">
+        <v>6.811628933434839</v>
+      </c>
+      <c r="AY8" t="n">
+        <v>8.307720445112523</v>
+      </c>
+      <c r="AZ8" t="n">
+        <v>12.7564172489878</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
@@ -1599,6 +1771,30 @@
       <c r="AR9" t="n">
         <v>0.9848144054412842</v>
       </c>
+      <c r="AS9" t="n">
+        <v>0.9997463822364807</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>0.9997308254241943</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>0.9997228384017944</v>
+      </c>
+      <c r="AV9" t="n">
+        <v>0.9996931552886963</v>
+      </c>
+      <c r="AW9" t="n">
+        <v>0.9996346831321716</v>
+      </c>
+      <c r="AX9" t="n">
+        <v>0.9995160102844238</v>
+      </c>
+      <c r="AY9" t="n">
+        <v>0.9991301894187927</v>
+      </c>
+      <c r="AZ9" t="n">
+        <v>0.9975930452346802</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1736,6 +1932,30 @@
       </c>
       <c r="AR10" t="n">
         <v>30.24324989318848</v>
+      </c>
+      <c r="AS10" t="n">
+        <v>3.59768009185791</v>
+      </c>
+      <c r="AT10" t="n">
+        <v>3.71510910987854</v>
+      </c>
+      <c r="AU10" t="n">
+        <v>3.809412479400635</v>
+      </c>
+      <c r="AV10" t="n">
+        <v>3.969744205474854</v>
+      </c>
+      <c r="AW10" t="n">
+        <v>4.085700988769531</v>
+      </c>
+      <c r="AX10" t="n">
+        <v>4.858162879943848</v>
+      </c>
+      <c r="AY10" t="n">
+        <v>5.752134323120117</v>
+      </c>
+      <c r="AZ10" t="n">
+        <v>9.018462181091309</v>
       </c>
     </row>
     <row r="11">
@@ -1871,6 +2091,30 @@
       <c r="AR11" t="n">
         <v>30.43869310739109</v>
       </c>
+      <c r="AS11" t="n">
+        <v>4.59340598965685</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>4.689419162790909</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>4.81294169194917</v>
+      </c>
+      <c r="AV11" t="n">
+        <v>5.024516462908163</v>
+      </c>
+      <c r="AW11" t="n">
+        <v>5.139634242718618</v>
+      </c>
+      <c r="AX11" t="n">
+        <v>6.112371387961876</v>
+      </c>
+      <c r="AY11" t="n">
+        <v>7.222035110527732</v>
+      </c>
+      <c r="AZ11" t="n">
+        <v>11.23793196309396</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
@@ -2005,9 +2249,33 @@
       <c r="AR12" t="n">
         <v>0.9872711896896362</v>
       </c>
+      <c r="AS12" t="n">
+        <v>0.9997574687004089</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>0.9997386932373047</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>0.9997255802154541</v>
+      </c>
+      <c r="AV12" t="n">
+        <v>0.9996883273124695</v>
+      </c>
+      <c r="AW12" t="n">
+        <v>0.9996572732925415</v>
+      </c>
+      <c r="AX12" t="n">
+        <v>0.9994662404060364</v>
+      </c>
+      <c r="AY12" t="n">
+        <v>0.9991978406906128</v>
+      </c>
+      <c r="AZ12" t="n">
+        <v>0.9978833198547363</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="M1:T1"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A9"/>
@@ -2016,6 +2284,7 @@
     <mergeCell ref="AC1:AJ1"/>
     <mergeCell ref="AK1:AR1"/>
     <mergeCell ref="U1:AB1"/>
+    <mergeCell ref="AS1:AZ1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>